<commit_message>
data for nutrient analysis
</commit_message>
<xml_diff>
--- a/NitrogenPhosphorous/DATA.hf_nutrients.xlsx
+++ b/NitrogenPhosphorous/DATA.hf_nutrients.xlsx
@@ -18,14 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">data!$D$2:$D$33</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">data!$F$2:$F$33</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">data!$E$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">data!$E$2:$E$33</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">data!$D$2:$D$33</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">data!$G$2:$G$33</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">data!$F$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">data!$F$2:$F$33</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">data!$D$2:$D$33</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">data!$E$2:$E$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">data!$G$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">data!$G$2:$G$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -303,10 +303,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -344,7 +344,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{0336CAD8-5EDC-2A41-9C94-2C75BD131DD8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>ammonium</cx:v>
             </cx:txData>
           </cx:tx>
@@ -374,10 +374,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -415,7 +415,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CA849EC5-3334-4145-A973-E7C855102ED8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>orthophosphate</cx:v>
             </cx:txData>
           </cx:tx>
@@ -445,10 +445,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -486,7 +486,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{67E246CD-1586-564D-850F-1FF3818A29AD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>nitrate</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3490,7 +3490,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>